<commit_message>
add  helper.go and template,but have bug. came back home fix
</commit_message>
<xml_diff>
--- a/conf/type/Item.xlsx
+++ b/conf/type/Item.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>种类</t>
   </si>
@@ -150,6 +150,10 @@
   </si>
   <si>
     <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,7 +555,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -606,7 +610,9 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>